<commit_message>
feat: Allow custom column count
- Validate column count arg type
</commit_message>
<xml_diff>
--- a/MCQs.xlsx
+++ b/MCQs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -509,6 +509,156 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This is the first question?
+</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">option a
+</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">option b
+</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">option c
+</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">option d
+</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">a
+</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The answer can be 'a' for now
+</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This is the first question?
+</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">option a
+</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">option b
+</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">option c
+</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">option d
+</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">a
+</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The answer can be 'a' for now
+</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This is the first question?
+</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">option a
+</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">option b
+</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">option c
+</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">option d
+</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">a
+</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The answer can be 'a' for now
+</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>